<commit_message>
Installed capacities 2022 Germany
</commit_message>
<xml_diff>
--- a/Operational/Germany_2022/Capacity.xlsx
+++ b/Operational/Germany_2022/Capacity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Desktop/Dummy Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/negarnamazifard/Documents/GitHub/ESM-Py/Operational/Germany_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA14DE33-D72B-084B-B16A-9A17D8B79A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFE8B44-451E-C546-B4BB-007B6DD02FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{FF9D44F2-6E08-3D4B-A906-FA3E1828E5C6}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="16420" xr2:uid="{FF9D44F2-6E08-3D4B-A906-FA3E1828E5C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,24 +34,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>PV</t>
-  </si>
-  <si>
-    <t>OIL</t>
-  </si>
-  <si>
-    <t>Capacity</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Installed Capacities year 2022</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Fossil Hard coal</t>
+  </si>
+  <si>
+    <t>Wind Onshore</t>
+  </si>
+  <si>
+    <t>Fossil Brown coal/Lignite</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>Hydro Run-of-river and poundage</t>
+  </si>
+  <si>
+    <t>Hydro Water Reservoir</t>
+  </si>
+  <si>
+    <t>Wind Offshore</t>
+  </si>
+  <si>
+    <t>Hydro Pumped Storage</t>
+  </si>
+  <si>
+    <t>Other renewable</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>Fossil Gas</t>
+  </si>
+  <si>
+    <t>Fossil Oil</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Total Grand capacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,31 +451,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EDDFEC-FA1A-A440-9D4C-A1DD859BFEF8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <v>60</v>
+      <c r="B3">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>18830</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>55797</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>19106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>7787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>9280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>56567</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>30649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>8590</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>223540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dmand FIle and Availablities
</commit_message>
<xml_diff>
--- a/Operational/Germany_2022/Capacity.xlsx
+++ b/Operational/Germany_2022/Capacity.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/negarnamazifard/Documents/GitHub/ESM-Py/Operational/Germany_2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/ESM-Py/Operational/Germany_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFE8B44-451E-C546-B4BB-007B6DD02FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AF500A-0EE3-6F46-844B-6DF40F067CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="16420" xr2:uid="{FF9D44F2-6E08-3D4B-A906-FA3E1828E5C6}"/>
+    <workbookView xWindow="2120" yWindow="2760" windowWidth="28040" windowHeight="16420" xr2:uid="{FF9D44F2-6E08-3D4B-A906-FA3E1828E5C6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,80 +34,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Installed Capacities year 2022</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Fossil Hard coal</t>
-  </si>
-  <si>
-    <t>Wind Onshore</t>
-  </si>
-  <si>
-    <t>Fossil Brown coal/Lignite</t>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>Hydro Run-of-river and poundage</t>
-  </si>
-  <si>
-    <t>Hydro Water Reservoir</t>
-  </si>
-  <si>
-    <t>Wind Offshore</t>
-  </si>
-  <si>
-    <t>Hydro Pumped Storage</t>
-  </si>
-  <si>
-    <t>Other renewable</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>Waste</t>
-  </si>
-  <si>
-    <t>Fossil Gas</t>
-  </si>
-  <si>
-    <t>Fossil Oil</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Biomass</t>
-  </si>
-  <si>
-    <t>Total Grand capacity</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Coal Power Plant</t>
+  </si>
+  <si>
+    <t>Nuclear Power Plant</t>
+  </si>
+  <si>
+    <t>Wind Power Plant</t>
+  </si>
+  <si>
+    <t>Geothermal Power Plant</t>
+  </si>
+  <si>
+    <t>Hydro Power Plant</t>
+  </si>
+  <si>
+    <t>Waste and Biomass</t>
+  </si>
+  <si>
+    <t>Gas Power Plants</t>
+  </si>
+  <si>
+    <t>Oil Power Plants</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Solar Power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -134,9 +99,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,160 +414,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EDDFEC-FA1A-A440-9D4C-A1DD859BFEF8}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A6782C-52EB-5447-B0A7-C3CFA3ACAF35}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H1" activeCellId="3" sqref="B1:C1 E1 F1 H1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>4056</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>18830</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>55797</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>19106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+      <c r="C2">
+        <v>37936</v>
+      </c>
+      <c r="D2">
+        <v>63584</v>
+      </c>
+      <c r="E2">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>3743</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>7787</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>9280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
+      <c r="F2">
+        <v>14431</v>
+      </c>
+      <c r="G2">
         <v>56567</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
+      <c r="H2">
+        <v>10210</v>
+      </c>
+      <c r="I2">
         <v>30649</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
+      <c r="J2">
         <v>3966</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>1679</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>8590</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>223540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>